<commit_message>
Texto pronto, agora é ensaiar
</commit_message>
<xml_diff>
--- a/Apresentação/Lista slides e tempo.xlsx
+++ b/Apresentação/Lista slides e tempo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Documents\Mestrado\Dissertação\Apresentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITA\Dissertacao\Apresentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09CBAA4-4D70-4213-BDA5-8470571399BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A62C94-FC81-4C80-80C8-5F4A20E1BAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -226,7 +225,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[mm]:ss"/>
+    <numFmt numFmtId="164" formatCode="[mm]:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -266,8 +265,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -553,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2663,21 +2662,24 @@
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
+      <c r="F56">
+        <v>37</v>
+      </c>
       <c r="G56">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>1939</v>
       </c>
       <c r="H56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="I56">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>32.31666666666667</v>
       </c>
       <c r="J56" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>32:19</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="2"/>
@@ -2698,21 +2700,24 @@
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
+      <c r="F57">
+        <v>29</v>
+      </c>
       <c r="G57">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>1968</v>
       </c>
       <c r="H57">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.48333333333333334</v>
       </c>
       <c r="I57">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="J57" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>32:47</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="2"/>
@@ -2733,21 +2738,24 @@
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
+      <c r="F58">
+        <v>56</v>
+      </c>
       <c r="G58">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2024</v>
       </c>
       <c r="H58">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="I58">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>33.733333333333334</v>
       </c>
       <c r="J58" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>33:44</v>
       </c>
       <c r="K58" t="str">
         <f t="shared" si="2"/>
@@ -2768,21 +2776,24 @@
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
+      <c r="F59">
+        <v>8</v>
+      </c>
       <c r="G59">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2032</v>
       </c>
       <c r="H59">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="I59">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>33.866666666666667</v>
       </c>
       <c r="J59" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>33:52</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="2"/>
@@ -2803,21 +2814,24 @@
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
+      <c r="F60">
+        <v>7</v>
+      </c>
       <c r="G60">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2039</v>
       </c>
       <c r="H60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.11666666666666667</v>
       </c>
       <c r="I60">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>33.983333333333334</v>
       </c>
       <c r="J60" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>33:59</v>
       </c>
       <c r="K60" t="str">
         <f t="shared" si="2"/>
@@ -2838,21 +2852,24 @@
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
+      <c r="F61">
+        <v>13</v>
+      </c>
       <c r="G61">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2052</v>
       </c>
       <c r="H61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I61">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="J61" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>34:12</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="2"/>
@@ -2873,21 +2890,24 @@
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
+      <c r="F62">
+        <v>25</v>
+      </c>
       <c r="G62">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2077</v>
       </c>
       <c r="H62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="I62">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>34.616666666666667</v>
       </c>
       <c r="J62" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>34:37</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="2"/>
@@ -2908,21 +2928,24 @@
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
+      <c r="F63">
+        <v>14</v>
+      </c>
       <c r="G63">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2091</v>
       </c>
       <c r="H63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.23333333333333334</v>
       </c>
       <c r="I63">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>34.85</v>
       </c>
       <c r="J63" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>34:51</v>
       </c>
       <c r="K63" t="str">
         <f t="shared" si="2"/>
@@ -2943,21 +2966,24 @@
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
+      <c r="F64">
+        <v>42</v>
+      </c>
       <c r="G64">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2133</v>
       </c>
       <c r="H64">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="I64">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>35.549999999999997</v>
       </c>
       <c r="J64" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>35:32</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" si="2"/>
@@ -2978,21 +3004,24 @@
         <f t="shared" si="4"/>
         <v>35</v>
       </c>
+      <c r="F65">
+        <v>25</v>
+      </c>
       <c r="G65">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2158</v>
       </c>
       <c r="H65">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="I65">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>35.966666666666669</v>
       </c>
       <c r="J65" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>35:58</v>
       </c>
       <c r="K65" t="str">
         <f t="shared" si="2"/>
@@ -3013,21 +3042,24 @@
         <f t="shared" si="4"/>
         <v>35</v>
       </c>
+      <c r="F66">
+        <v>20</v>
+      </c>
       <c r="G66">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2178</v>
       </c>
       <c r="H66">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I66">
         <f t="shared" si="0"/>
-        <v>31.7</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="J66" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>31:42</v>
+        <v>36:17</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="2"/>
@@ -3048,21 +3080,24 @@
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
+      <c r="F67">
+        <v>13</v>
+      </c>
       <c r="G67">
         <f t="shared" si="3"/>
-        <v>1902</v>
+        <v>2191</v>
       </c>
       <c r="H67">
         <f t="shared" ref="H67:I90" si="5">F67/60</f>
-        <v>0</v>
+        <v>0.21666666666666667</v>
       </c>
       <c r="I67">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>36.516666666666666</v>
       </c>
       <c r="J67" s="2" t="str">
         <f t="shared" ref="J67:J90" si="6">INT(I67)&amp;":"&amp;INT((I67-INT(I67))*60)</f>
-        <v>31:42</v>
+        <v>36:30</v>
       </c>
       <c r="K67" t="str">
         <f t="shared" ref="K67:K90" si="7">INT($A$2*B67)&amp;":"&amp;TEXT(INT(($A$2*B67-INT($A$2*B67))*60),0)</f>
@@ -3083,21 +3118,24 @@
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
+      <c r="F68">
+        <v>20</v>
+      </c>
       <c r="G68">
         <f t="shared" ref="G68:G90" si="8">F68+G67</f>
-        <v>1902</v>
+        <v>2211</v>
       </c>
       <c r="H68">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I68">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>36.85</v>
       </c>
       <c r="J68" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>36:51</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="7"/>
@@ -3118,21 +3156,24 @@
         <f t="shared" ref="E69:E90" si="9">IF(NOT(OR(C69="Capa",C69="Agenda",C69="Final",D69=D68)),E68+1,E68+0)</f>
         <v>37</v>
       </c>
+      <c r="F69">
+        <v>20</v>
+      </c>
       <c r="G69">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2231</v>
       </c>
       <c r="H69">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I69">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>37.18333333333333</v>
       </c>
       <c r="J69" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>37:10</v>
       </c>
       <c r="K69" t="str">
         <f t="shared" si="7"/>
@@ -3153,21 +3194,24 @@
         <f t="shared" si="9"/>
         <v>37</v>
       </c>
+      <c r="F70">
+        <v>20</v>
+      </c>
       <c r="G70">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2251</v>
       </c>
       <c r="H70">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I70">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>37.516666666666666</v>
       </c>
       <c r="J70" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>37:30</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="7"/>
@@ -3188,21 +3232,24 @@
         <f t="shared" si="9"/>
         <v>37</v>
       </c>
+      <c r="F71">
+        <v>20</v>
+      </c>
       <c r="G71">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2271</v>
       </c>
       <c r="H71">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I71">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>37.85</v>
       </c>
       <c r="J71" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>37:51</v>
       </c>
       <c r="K71" t="str">
         <f t="shared" si="7"/>
@@ -3223,21 +3270,24 @@
         <f t="shared" si="9"/>
         <v>38</v>
       </c>
+      <c r="F72">
+        <v>20</v>
+      </c>
       <c r="G72">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2291</v>
       </c>
       <c r="H72">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I72">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>38.18333333333333</v>
       </c>
       <c r="J72" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>38:10</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" si="7"/>
@@ -3258,21 +3308,24 @@
         <f t="shared" si="9"/>
         <v>38</v>
       </c>
+      <c r="F73">
+        <v>10</v>
+      </c>
       <c r="G73">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2301</v>
       </c>
       <c r="H73">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I73">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>38.35</v>
       </c>
       <c r="J73" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>38:21</v>
       </c>
       <c r="K73" t="str">
         <f t="shared" si="7"/>
@@ -3293,21 +3346,24 @@
         <f t="shared" si="9"/>
         <v>39</v>
       </c>
+      <c r="F74">
+        <v>12</v>
+      </c>
       <c r="G74">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2313</v>
       </c>
       <c r="H74">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I74">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>38.549999999999997</v>
       </c>
       <c r="J74" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>38:32</v>
       </c>
       <c r="K74" t="str">
         <f t="shared" si="7"/>
@@ -3328,21 +3384,24 @@
         <f t="shared" si="9"/>
         <v>39</v>
       </c>
+      <c r="F75">
+        <v>23</v>
+      </c>
       <c r="G75">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2336</v>
       </c>
       <c r="H75">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.38333333333333336</v>
       </c>
       <c r="I75">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>38.93333333333333</v>
       </c>
       <c r="J75" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>38:55</v>
       </c>
       <c r="K75" t="str">
         <f t="shared" si="7"/>
@@ -3363,21 +3422,24 @@
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
+      <c r="F76">
+        <v>20</v>
+      </c>
       <c r="G76">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2356</v>
       </c>
       <c r="H76">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I76">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>39.266666666666666</v>
       </c>
       <c r="J76" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>39:15</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" si="7"/>
@@ -3398,21 +3460,24 @@
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
+      <c r="F77">
+        <v>25</v>
+      </c>
       <c r="G77">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2381</v>
       </c>
       <c r="H77">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="I77">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>39.68333333333333</v>
       </c>
       <c r="J77" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>39:40</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="7"/>
@@ -3433,21 +3498,24 @@
         <f t="shared" si="9"/>
         <v>41</v>
       </c>
+      <c r="F78">
+        <v>20</v>
+      </c>
       <c r="G78">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2401</v>
       </c>
       <c r="H78">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I78">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>40.016666666666666</v>
       </c>
       <c r="J78" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>40:0</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="7"/>
@@ -3468,21 +3536,24 @@
         <f t="shared" si="9"/>
         <v>41</v>
       </c>
+      <c r="F79">
+        <v>27</v>
+      </c>
       <c r="G79">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2428</v>
       </c>
       <c r="H79">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="I79">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>40.466666666666669</v>
       </c>
       <c r="J79" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>40:28</v>
       </c>
       <c r="K79" t="str">
         <f t="shared" si="7"/>
@@ -3503,21 +3574,24 @@
         <f t="shared" si="9"/>
         <v>41</v>
       </c>
+      <c r="F80">
+        <v>25</v>
+      </c>
       <c r="G80">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2453</v>
       </c>
       <c r="H80">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="I80">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>40.883333333333333</v>
       </c>
       <c r="J80" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>40:53</v>
       </c>
       <c r="K80" t="str">
         <f t="shared" si="7"/>
@@ -3538,21 +3612,24 @@
         <f t="shared" si="9"/>
         <v>41</v>
       </c>
+      <c r="F81">
+        <v>36</v>
+      </c>
       <c r="G81">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2489</v>
       </c>
       <c r="H81">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I81">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>41.483333333333334</v>
       </c>
       <c r="J81" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>41:29</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="7"/>
@@ -3573,9 +3650,12 @@
         <f t="shared" si="9"/>
         <v>41</v>
       </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
       <c r="G82">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2489</v>
       </c>
       <c r="H82">
         <f t="shared" si="5"/>
@@ -3583,11 +3663,11 @@
       </c>
       <c r="I82">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>41.483333333333334</v>
       </c>
       <c r="J82" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>41:29</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="7"/>
@@ -3608,21 +3688,24 @@
         <f t="shared" si="9"/>
         <v>42</v>
       </c>
+      <c r="F83">
+        <v>116</v>
+      </c>
       <c r="G83">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2605</v>
       </c>
       <c r="H83">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.9333333333333333</v>
       </c>
       <c r="I83">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>43.416666666666664</v>
       </c>
       <c r="J83" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>43:24</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="7"/>
@@ -3643,21 +3726,24 @@
         <f t="shared" si="9"/>
         <v>42</v>
       </c>
+      <c r="F84">
+        <v>45</v>
+      </c>
       <c r="G84">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2650</v>
       </c>
       <c r="H84">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I84">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>44.166666666666664</v>
       </c>
       <c r="J84" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>44:9</v>
       </c>
       <c r="K84" t="str">
         <f t="shared" si="7"/>
@@ -3678,21 +3764,24 @@
         <f t="shared" si="9"/>
         <v>43</v>
       </c>
+      <c r="F85">
+        <v>17</v>
+      </c>
       <c r="G85">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2667</v>
       </c>
       <c r="H85">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.28333333333333333</v>
       </c>
       <c r="I85">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>44.45</v>
       </c>
       <c r="J85" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>44:27</v>
       </c>
       <c r="K85" t="str">
         <f t="shared" si="7"/>
@@ -3713,21 +3802,24 @@
         <f t="shared" si="9"/>
         <v>43</v>
       </c>
+      <c r="F86">
+        <v>11</v>
+      </c>
       <c r="G86">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2678</v>
       </c>
       <c r="H86">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.18333333333333332</v>
       </c>
       <c r="I86">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>44.633333333333333</v>
       </c>
       <c r="J86" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>44:38</v>
       </c>
       <c r="K86" t="str">
         <f t="shared" si="7"/>
@@ -3748,21 +3840,24 @@
         <f t="shared" si="9"/>
         <v>43</v>
       </c>
+      <c r="F87">
+        <v>8</v>
+      </c>
       <c r="G87">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2686</v>
       </c>
       <c r="H87">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="I87">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>44.766666666666666</v>
       </c>
       <c r="J87" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>44:45</v>
       </c>
       <c r="K87" t="str">
         <f t="shared" si="7"/>
@@ -3783,21 +3878,24 @@
         <f t="shared" si="9"/>
         <v>43</v>
       </c>
+      <c r="F88">
+        <v>10</v>
+      </c>
       <c r="G88">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2696</v>
       </c>
       <c r="H88">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I88">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>44.93333333333333</v>
       </c>
       <c r="J88" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>44:55</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="7"/>
@@ -3818,21 +3916,24 @@
         <f t="shared" si="9"/>
         <v>43</v>
       </c>
+      <c r="F89">
+        <v>10</v>
+      </c>
       <c r="G89">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2706</v>
       </c>
       <c r="H89">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I89">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>45.1</v>
       </c>
       <c r="J89" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>45:6</v>
       </c>
       <c r="K89" t="str">
         <f t="shared" si="7"/>
@@ -3853,21 +3954,24 @@
         <f t="shared" si="9"/>
         <v>43</v>
       </c>
+      <c r="F90">
+        <v>10</v>
+      </c>
       <c r="G90">
         <f t="shared" si="8"/>
-        <v>1902</v>
+        <v>2716</v>
       </c>
       <c r="H90">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I90">
         <f t="shared" si="5"/>
-        <v>31.7</v>
+        <v>45.266666666666666</v>
       </c>
       <c r="J90" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>31:42</v>
+        <v>45:15</v>
       </c>
       <c r="K90" t="str">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
Acho que agora acabou
</commit_message>
<xml_diff>
--- a/Apresentação/Lista slides e tempo.xlsx
+++ b/Apresentação/Lista slides e tempo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Documents\Mestrado\Dissertação\Apresentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITA\Dissertacao\Apresentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57432D5F-3312-4A7B-9766-8543C7938193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B984CC-E15B-4449-8516-6933A02082C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -253,6 +253,7 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1048575"/>
+  <dimension ref="A1:P1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +547,7 @@
     <col min="10" max="10" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>30</v>
       </c>
@@ -572,7 +573,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>50/COUNT(B2:B89)</f>
         <v>0.56818181818181823</v>
@@ -614,7 +615,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2*60</f>
         <v>34.090909090909093</v>
@@ -648,11 +649,11 @@
         <v>0.6</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J16" si="1">INT(I3)&amp;":"&amp;INT((I3-INT(I3))*60)</f>
+        <f t="shared" ref="J3:J66" si="1">INT(I3)&amp;":"&amp;INT((I3-INT(I3))*60)</f>
         <v>0:36</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K65" si="2">INT($A$2*B3)&amp;":"&amp;TEXT(INT(($A$2*B3-INT($A$2*B3))*60),0)</f>
+        <f t="shared" ref="K3:K66" si="2">INT($A$2*B3)&amp;":"&amp;TEXT(INT(($A$2*B3-INT($A$2*B3))*60),0)</f>
         <v>1:8</v>
       </c>
       <c r="L3" s="4"/>
@@ -663,7 +664,7 @@
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -693,7 +694,7 @@
         <v>1.35</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f t="shared" ref="J4:J7" si="6">INT(I4)&amp;":"&amp;INT((I4-INT(I4))*60)</f>
+        <f t="shared" si="1"/>
         <v>1:21</v>
       </c>
       <c r="K4" t="str">
@@ -707,8 +708,12 @@
       <c r="N4" s="4">
         <v>2.361111111111111E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="4">
+        <f>N4-N3</f>
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -738,7 +743,7 @@
         <v>1.4333333333333333</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1:26</v>
       </c>
       <c r="K5" t="str">
@@ -752,8 +757,12 @@
       <c r="N5" s="4">
         <v>7.2222222222222229E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="4">
+        <f t="shared" ref="O5:O63" si="6">N5-N4</f>
+        <v>4.8611111111111119E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -783,7 +792,7 @@
         <v>1.5166666666666666</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f t="shared" ref="J6" si="9">INT(I6)&amp;":"&amp;INT((I6-INT(I6))*60)</f>
+        <f t="shared" si="1"/>
         <v>1:31</v>
       </c>
       <c r="K6" t="str">
@@ -797,8 +806,12 @@
       <c r="N6" s="4">
         <v>7.7083333333333337E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="4">
+        <f t="shared" si="6"/>
+        <v>4.8611111111111077E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -828,7 +841,7 @@
         <v>1.75</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1:45</v>
       </c>
       <c r="K7" t="str">
@@ -838,8 +851,12 @@
       <c r="N7" s="4">
         <v>8.1250000000000003E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="4">
+        <f t="shared" si="6"/>
+        <v>4.1666666666666657E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -883,8 +900,12 @@
       <c r="N8" s="4">
         <v>8.819444444444445E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="4">
+        <f t="shared" si="6"/>
+        <v>6.9444444444444475E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
@@ -926,8 +947,12 @@
       <c r="N9" s="4">
         <v>9.375E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="4">
+        <f t="shared" si="6"/>
+        <v>5.5555555555555497E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
@@ -967,8 +992,12 @@
       <c r="N10" s="4">
         <v>0.10208333333333335</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="4">
+        <f t="shared" si="6"/>
+        <v>8.3333333333333454E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
@@ -1008,8 +1037,12 @@
       <c r="N11" s="4">
         <v>0.10902777777777778</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="4">
+        <f t="shared" si="6"/>
+        <v>6.9444444444444337E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>11</v>
       </c>
@@ -1053,8 +1086,12 @@
       <c r="N12" s="4">
         <v>0.13263888888888889</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="4">
+        <f t="shared" si="6"/>
+        <v>2.361111111111111E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>12</v>
       </c>
@@ -1095,8 +1132,12 @@
       <c r="N13" s="4">
         <v>0.19166666666666665</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="4">
+        <f t="shared" si="6"/>
+        <v>5.9027777777777762E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>13</v>
       </c>
@@ -1126,7 +1167,7 @@
         <v>5.5</v>
       </c>
       <c r="J14" s="2" t="str">
-        <f>INT(I14)&amp;":"&amp;INT((I14-INT(I14))*60)</f>
+        <f t="shared" si="1"/>
         <v>5:30</v>
       </c>
       <c r="K14" t="str">
@@ -1137,8 +1178,12 @@
         <v>0.26458333333333334</v>
       </c>
       <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.19166666666666665</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>14</v>
       </c>
@@ -1179,8 +1224,12 @@
       <c r="N15" s="4">
         <v>0.2673611111111111</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="4">
+        <f t="shared" si="6"/>
+        <v>0.2673611111111111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>15</v>
       </c>
@@ -1220,8 +1269,12 @@
       <c r="N16" s="4">
         <v>0.29305555555555557</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="4">
+        <f t="shared" si="6"/>
+        <v>2.5694444444444464E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>16</v>
       </c>
@@ -1243,15 +1296,15 @@
         <v>393</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:H18" si="10">F17/60</f>
+        <f t="shared" ref="H17:H18" si="9">F17/60</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:I18" si="11">G17/60</f>
+        <f t="shared" ref="I17:I18" si="10">G17/60</f>
         <v>6.55</v>
       </c>
       <c r="J17" s="2" t="str">
-        <f t="shared" ref="J17:J18" si="12">INT(I17)&amp;":"&amp;INT((I17-INT(I17))*60)</f>
+        <f t="shared" si="1"/>
         <v>6:33</v>
       </c>
       <c r="K17" t="str">
@@ -1261,8 +1314,12 @@
       <c r="N17" s="4">
         <v>0.31597222222222221</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="4">
+        <f t="shared" si="6"/>
+        <v>2.2916666666666641E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>17</v>
       </c>
@@ -1273,7 +1330,7 @@
         <v>9</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:E81" si="13">IF(NOT(OR(C18="Agenda",C18="Final",D18=D17)),E17+1,E17+0)</f>
+        <f t="shared" ref="E18:E81" si="11">IF(NOT(OR(C18="Agenda",C18="Final",D18=D17)),E17+1,E17+0)</f>
         <v>8</v>
       </c>
       <c r="F18">
@@ -1284,23 +1341,30 @@
         <v>393</v>
       </c>
       <c r="H18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="11"/>
         <v>6.55</v>
       </c>
       <c r="J18" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="1"/>
         <v>6:33</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="2"/>
         <v>9:39</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.31597222222222221</v>
+      </c>
+      <c r="P18" s="4">
+        <v>0.30624999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>18</v>
       </c>
@@ -1311,7 +1375,7 @@
         <v>10</v>
       </c>
       <c r="E19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="F19">
@@ -1322,15 +1386,15 @@
         <v>468</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:H81" si="14">F19/60</f>
+        <f t="shared" ref="H19:H81" si="12">F19/60</f>
         <v>1.25</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:I81" si="15">G19/60</f>
+        <f t="shared" ref="I19:I81" si="13">G19/60</f>
         <v>7.8</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" ref="J19:J81" si="16">INT(I19)&amp;":"&amp;INT((I19-INT(I19))*60)</f>
+        <f t="shared" si="1"/>
         <v>7:48</v>
       </c>
       <c r="K19" t="str">
@@ -1340,8 +1404,13 @@
       <c r="N19" s="4">
         <v>0.32083333333333336</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="4">
+        <f t="shared" si="6"/>
+        <v>0.32083333333333336</v>
+      </c>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>19</v>
       </c>
@@ -1352,7 +1421,7 @@
         <v>11</v>
       </c>
       <c r="E20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="F20">
@@ -1363,15 +1432,15 @@
         <v>498</v>
       </c>
       <c r="H20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
       <c r="I20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="J20" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>8:18</v>
       </c>
       <c r="K20" t="str">
@@ -1381,8 +1450,12 @@
       <c r="N20" s="4">
         <v>0.37222222222222223</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="4">
+        <f t="shared" si="6"/>
+        <v>5.1388888888888873E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>20</v>
       </c>
@@ -1393,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="E21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="F21">
@@ -1404,15 +1477,15 @@
         <v>498</v>
       </c>
       <c r="H21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="J21" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>8:18</v>
       </c>
       <c r="K21" t="str">
@@ -1425,8 +1498,15 @@
       <c r="N21" s="4">
         <v>0.41180555555555554</v>
       </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="4">
+        <f t="shared" si="6"/>
+        <v>3.9583333333333304E-2</v>
+      </c>
+      <c r="P21" s="4">
+        <v>0.39999999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>21</v>
       </c>
@@ -1437,7 +1517,7 @@
         <v>14</v>
       </c>
       <c r="E22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="F22">
@@ -1448,15 +1528,15 @@
         <v>512</v>
       </c>
       <c r="H22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.23333333333333334</v>
       </c>
       <c r="I22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>8.5333333333333332</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>8:32</v>
       </c>
       <c r="K22" t="str">
@@ -1466,8 +1546,12 @@
       <c r="N22" s="4">
         <v>0.42708333333333331</v>
       </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="4">
+        <f t="shared" si="6"/>
+        <v>1.5277777777777779E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>22</v>
       </c>
@@ -1478,7 +1562,7 @@
         <v>15</v>
       </c>
       <c r="E23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="F23">
@@ -1489,15 +1573,15 @@
         <v>546</v>
       </c>
       <c r="H23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.56666666666666665</v>
       </c>
       <c r="I23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>9.1</v>
       </c>
       <c r="J23" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>9:5</v>
       </c>
       <c r="K23" t="str">
@@ -1507,8 +1591,12 @@
       <c r="N23" s="4">
         <v>0.4458333333333333</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="4">
+        <f t="shared" si="6"/>
+        <v>1.8749999999999989E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>23</v>
       </c>
@@ -1519,7 +1607,7 @@
         <v>16</v>
       </c>
       <c r="E24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="F24">
@@ -1530,23 +1618,27 @@
         <v>573</v>
       </c>
       <c r="H24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.45</v>
       </c>
       <c r="I24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>9.5500000000000007</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>9:33</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="2"/>
         <v>13:4</v>
       </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.4458333333333333</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>24</v>
       </c>
@@ -1557,7 +1649,7 @@
         <v>17</v>
       </c>
       <c r="E25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
       <c r="F25">
@@ -1568,23 +1660,27 @@
         <v>591</v>
       </c>
       <c r="H25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.3</v>
       </c>
       <c r="I25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>9.85</v>
       </c>
       <c r="J25" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>9:51</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="2"/>
         <v>13:38</v>
       </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>25</v>
       </c>
@@ -1595,7 +1691,7 @@
         <v>18</v>
       </c>
       <c r="E26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
       <c r="F26">
@@ -1606,23 +1702,27 @@
         <v>619</v>
       </c>
       <c r="H26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.46666666666666667</v>
       </c>
       <c r="I26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>10.316666666666666</v>
       </c>
       <c r="J26" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>10:19</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="2"/>
         <v>14:12</v>
       </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>26</v>
       </c>
@@ -1633,7 +1733,7 @@
         <v>19</v>
       </c>
       <c r="E27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="F27">
@@ -1644,15 +1744,15 @@
         <v>668</v>
       </c>
       <c r="H27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.81666666666666665</v>
       </c>
       <c r="I27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>11.133333333333333</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>11:7</v>
       </c>
       <c r="K27" t="str">
@@ -1662,8 +1762,12 @@
       <c r="N27" s="4">
         <v>0.4909722222222222</v>
       </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="4">
+        <f t="shared" si="6"/>
+        <v>0.4909722222222222</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>27</v>
       </c>
@@ -1674,7 +1778,7 @@
         <v>20</v>
       </c>
       <c r="E28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>17</v>
       </c>
       <c r="F28">
@@ -1686,15 +1790,15 @@
         <v>750</v>
       </c>
       <c r="H28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1.3666666666666667</v>
       </c>
       <c r="I28">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>12.5</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>12:30</v>
       </c>
       <c r="K28" t="str">
@@ -1704,8 +1808,12 @@
       <c r="N28" s="4">
         <v>0.52638888888888891</v>
       </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="4">
+        <f t="shared" si="6"/>
+        <v>3.5416666666666707E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>28</v>
       </c>
@@ -1716,7 +1824,7 @@
         <v>21</v>
       </c>
       <c r="E29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>18</v>
       </c>
       <c r="F29">
@@ -1728,15 +1836,15 @@
         <v>825</v>
       </c>
       <c r="H29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1.25</v>
       </c>
       <c r="I29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>13.75</v>
       </c>
       <c r="J29" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>13:45</v>
       </c>
       <c r="K29" t="str">
@@ -1749,8 +1857,12 @@
       <c r="N29" s="4">
         <v>0.58958333333333335</v>
       </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="4">
+        <f t="shared" si="6"/>
+        <v>6.3194444444444442E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>29</v>
       </c>
@@ -1761,7 +1873,7 @@
         <v>22</v>
       </c>
       <c r="E30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="F30">
@@ -1772,15 +1884,15 @@
         <v>876</v>
       </c>
       <c r="H30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.85</v>
       </c>
       <c r="I30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>14.6</v>
       </c>
       <c r="J30" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>14:36</v>
       </c>
       <c r="K30" t="str">
@@ -1790,8 +1902,12 @@
       <c r="N30" s="4">
         <v>0.65833333333333333</v>
       </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="4">
+        <f t="shared" si="6"/>
+        <v>6.8749999999999978E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>30</v>
       </c>
@@ -1802,7 +1918,7 @@
         <v>23</v>
       </c>
       <c r="E31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>20</v>
       </c>
       <c r="F31">
@@ -1813,15 +1929,15 @@
         <v>908</v>
       </c>
       <c r="H31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="I31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>15.133333333333333</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>15:7</v>
       </c>
       <c r="K31" t="str">
@@ -1831,8 +1947,12 @@
       <c r="N31" s="4">
         <v>0.69305555555555554</v>
       </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="4">
+        <f t="shared" si="6"/>
+        <v>3.472222222222221E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>31</v>
       </c>
@@ -1843,7 +1963,7 @@
         <v>24</v>
       </c>
       <c r="E32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
       <c r="F32">
@@ -1854,15 +1974,15 @@
         <v>938</v>
       </c>
       <c r="H32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
       <c r="I32">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>15.633333333333333</v>
       </c>
       <c r="J32" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>15:38</v>
       </c>
       <c r="K32" t="str">
@@ -1872,8 +1992,12 @@
       <c r="N32" s="4">
         <v>0.72777777777777775</v>
       </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O32" s="4">
+        <f t="shared" si="6"/>
+        <v>3.472222222222221E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>32</v>
       </c>
@@ -1884,7 +2008,7 @@
         <v>25</v>
       </c>
       <c r="E33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>22</v>
       </c>
       <c r="F33">
@@ -1895,15 +2019,15 @@
         <v>998</v>
       </c>
       <c r="H33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="I33">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>16.633333333333333</v>
       </c>
       <c r="J33" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>16:38</v>
       </c>
       <c r="K33" t="str">
@@ -1913,8 +2037,12 @@
       <c r="N33" s="4">
         <v>0.76944444444444438</v>
       </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O33" s="4">
+        <f t="shared" si="6"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>33</v>
       </c>
@@ -1925,7 +2053,7 @@
         <v>26</v>
       </c>
       <c r="E34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>22</v>
       </c>
       <c r="F34">
@@ -1936,15 +2064,15 @@
         <v>998</v>
       </c>
       <c r="H34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>16.633333333333333</v>
       </c>
       <c r="J34" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>16:38</v>
       </c>
       <c r="K34" t="str">
@@ -1954,8 +2082,15 @@
       <c r="N34" s="4">
         <v>0.81180555555555556</v>
       </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="4">
+        <f t="shared" si="6"/>
+        <v>4.2361111111111183E-2</v>
+      </c>
+      <c r="P34" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>34</v>
       </c>
@@ -1966,7 +2101,7 @@
         <v>27</v>
       </c>
       <c r="E35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>23</v>
       </c>
       <c r="F35">
@@ -1977,15 +2112,15 @@
         <v>1022</v>
       </c>
       <c r="H35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.4</v>
       </c>
       <c r="I35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>17.033333333333335</v>
       </c>
       <c r="J35" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>17:2</v>
       </c>
       <c r="K35" t="str">
@@ -1993,8 +2128,12 @@
         <v>19:19</v>
       </c>
       <c r="N35" s="4"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.81180555555555556</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>35</v>
       </c>
@@ -2005,7 +2144,7 @@
         <v>28</v>
       </c>
       <c r="E36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>24</v>
       </c>
       <c r="F36">
@@ -2016,15 +2155,15 @@
         <v>1074</v>
       </c>
       <c r="H36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.8666666666666667</v>
       </c>
       <c r="I36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>17.899999999999999</v>
       </c>
       <c r="J36" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>17:53</v>
       </c>
       <c r="K36" t="str">
@@ -2034,8 +2173,12 @@
       <c r="N36" s="4">
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="4">
+        <f t="shared" si="6"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>36</v>
       </c>
@@ -2046,7 +2189,7 @@
         <v>29</v>
       </c>
       <c r="E37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
       <c r="F37">
@@ -2057,15 +2200,15 @@
         <v>1109</v>
       </c>
       <c r="H37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.58333333333333337</v>
       </c>
       <c r="I37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>18.483333333333334</v>
       </c>
       <c r="J37" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>18:29</v>
       </c>
       <c r="K37" t="str">
@@ -2075,8 +2218,12 @@
       <c r="N37" s="4">
         <v>0.86597222222222225</v>
       </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="4">
+        <f t="shared" si="6"/>
+        <v>3.2638888888888884E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>37</v>
       </c>
@@ -2087,7 +2234,7 @@
         <v>30</v>
       </c>
       <c r="E38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>26</v>
       </c>
       <c r="F38">
@@ -2098,15 +2245,15 @@
         <v>1125</v>
       </c>
       <c r="H38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="I38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>18.75</v>
       </c>
       <c r="J38" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>18:45</v>
       </c>
       <c r="K38" t="str">
@@ -2116,8 +2263,12 @@
       <c r="N38" s="4">
         <v>0.87986111111111109</v>
       </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="4">
+        <f t="shared" si="6"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>38</v>
       </c>
@@ -2128,7 +2279,7 @@
         <v>31</v>
       </c>
       <c r="E39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>27</v>
       </c>
       <c r="F39">
@@ -2139,15 +2290,15 @@
         <v>1157</v>
       </c>
       <c r="H39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="I39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>19.283333333333335</v>
       </c>
       <c r="J39" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>19:17</v>
       </c>
       <c r="K39" t="str">
@@ -2157,8 +2308,12 @@
       <c r="N39" s="4">
         <v>0.9194444444444444</v>
       </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="4">
+        <f t="shared" si="6"/>
+        <v>3.9583333333333304E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>39</v>
       </c>
@@ -2169,7 +2324,7 @@
         <v>32</v>
       </c>
       <c r="E40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>28</v>
       </c>
       <c r="F40">
@@ -2180,23 +2335,27 @@
         <v>1171</v>
       </c>
       <c r="H40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.23333333333333334</v>
       </c>
       <c r="I40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>19.516666666666666</v>
       </c>
       <c r="J40" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>19:30</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="2"/>
         <v>22:9</v>
       </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.9194444444444444</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>40</v>
       </c>
@@ -2207,7 +2366,7 @@
         <v>33</v>
       </c>
       <c r="E41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>29</v>
       </c>
       <c r="F41">
@@ -2218,23 +2377,27 @@
         <v>1183</v>
       </c>
       <c r="H41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
       <c r="I41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>19.716666666666665</v>
       </c>
       <c r="J41" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>19:42</v>
       </c>
       <c r="K41" t="str">
         <f t="shared" si="2"/>
         <v>22:43</v>
       </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>41</v>
       </c>
@@ -2245,7 +2408,7 @@
         <v>34</v>
       </c>
       <c r="E42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>30</v>
       </c>
       <c r="F42">
@@ -2256,23 +2419,27 @@
         <v>1211</v>
       </c>
       <c r="H42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.46666666666666667</v>
       </c>
       <c r="I42">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>20.183333333333334</v>
       </c>
       <c r="J42" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>20:11</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="2"/>
         <v>23:17</v>
       </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>42</v>
       </c>
@@ -2283,7 +2450,7 @@
         <v>35</v>
       </c>
       <c r="E43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>31</v>
       </c>
       <c r="F43">
@@ -2294,15 +2461,15 @@
         <v>1224</v>
       </c>
       <c r="H43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.21666666666666667</v>
       </c>
       <c r="I43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>20.399999999999999</v>
       </c>
       <c r="J43" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>20:23</v>
       </c>
       <c r="K43" t="str">
@@ -2312,8 +2479,12 @@
       <c r="N43" s="4">
         <v>0.95833333333333337</v>
       </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="4">
+        <f t="shared" si="6"/>
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>43</v>
       </c>
@@ -2324,7 +2495,7 @@
         <v>36</v>
       </c>
       <c r="E44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
       <c r="F44">
@@ -2335,23 +2506,27 @@
         <v>1254</v>
       </c>
       <c r="H44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
       <c r="I44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>20.9</v>
       </c>
       <c r="J44" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>20:53</v>
       </c>
       <c r="K44" t="str">
         <f t="shared" si="2"/>
         <v>24:25</v>
       </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>44</v>
       </c>
@@ -2362,7 +2537,7 @@
         <v>37</v>
       </c>
       <c r="E45">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>33</v>
       </c>
       <c r="F45">
@@ -2373,24 +2548,30 @@
         <v>1286</v>
       </c>
       <c r="H45">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="I45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>21.433333333333334</v>
       </c>
       <c r="J45" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>21:26</v>
       </c>
       <c r="K45" t="str">
         <f t="shared" si="2"/>
         <v>25:0</v>
       </c>
-      <c r="N45" s="4"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N45" s="4">
+        <v>0.98402777777777783</v>
+      </c>
+      <c r="O45" s="4">
+        <f t="shared" si="6"/>
+        <v>0.98402777777777783</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>45</v>
       </c>
@@ -2401,7 +2582,7 @@
         <v>38</v>
       </c>
       <c r="E46">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>34</v>
       </c>
       <c r="F46">
@@ -2412,23 +2593,30 @@
         <v>1317</v>
       </c>
       <c r="H46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.51666666666666672</v>
       </c>
       <c r="I46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>21.95</v>
       </c>
       <c r="J46" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>21:57</v>
       </c>
       <c r="K46" t="str">
         <f t="shared" si="2"/>
         <v>25:34</v>
       </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.98402777777777783</v>
+      </c>
+      <c r="P46">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>46</v>
       </c>
@@ -2439,7 +2627,7 @@
         <v>39</v>
       </c>
       <c r="E47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
       <c r="F47">
@@ -2450,23 +2638,27 @@
         <v>1330</v>
       </c>
       <c r="H47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.21666666666666667</v>
       </c>
       <c r="I47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22.166666666666668</v>
       </c>
       <c r="J47" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>22:10</v>
       </c>
       <c r="K47" t="str">
         <f t="shared" si="2"/>
         <v>26:8</v>
       </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>47</v>
       </c>
@@ -2477,7 +2669,7 @@
         <v>40</v>
       </c>
       <c r="E48">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>36</v>
       </c>
       <c r="F48">
@@ -2488,23 +2680,27 @@
         <v>1340</v>
       </c>
       <c r="H48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="I48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22.333333333333332</v>
       </c>
       <c r="J48" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>22:19</v>
       </c>
       <c r="K48" t="str">
         <f t="shared" si="2"/>
         <v>26:42</v>
       </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="O48" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>48</v>
       </c>
@@ -2515,7 +2711,7 @@
         <v>41</v>
       </c>
       <c r="E49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>37</v>
       </c>
       <c r="F49">
@@ -2526,23 +2722,27 @@
         <v>1358</v>
       </c>
       <c r="H49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.3</v>
       </c>
       <c r="I49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22.633333333333333</v>
       </c>
       <c r="J49" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>22:38</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="2"/>
         <v>27:16</v>
       </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="O49" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>49</v>
       </c>
@@ -2553,7 +2753,7 @@
         <v>42</v>
       </c>
       <c r="E50">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>38</v>
       </c>
       <c r="F50">
@@ -2564,23 +2764,30 @@
         <v>1366</v>
       </c>
       <c r="H50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.13333333333333333</v>
       </c>
       <c r="I50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22.766666666666666</v>
       </c>
       <c r="J50" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>22:45</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="2"/>
         <v>27:50</v>
       </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="O50" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>50</v>
       </c>
@@ -2591,7 +2798,7 @@
         <v>43</v>
       </c>
       <c r="E51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>39</v>
       </c>
       <c r="F51">
@@ -2602,23 +2809,27 @@
         <v>1392</v>
       </c>
       <c r="H51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.43333333333333335</v>
       </c>
       <c r="I51">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23.2</v>
       </c>
       <c r="J51" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>23:12</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="2"/>
         <v>28:24</v>
       </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="O51" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>51</v>
       </c>
@@ -2629,7 +2840,7 @@
         <v>44</v>
       </c>
       <c r="E52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="F52">
@@ -2640,23 +2851,30 @@
         <v>1429</v>
       </c>
       <c r="H52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.6166666666666667</v>
       </c>
       <c r="I52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23.816666666666666</v>
       </c>
       <c r="J52" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>23:49</v>
       </c>
       <c r="K52" t="str">
         <f t="shared" si="2"/>
         <v>28:58</v>
       </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N52" s="5">
+        <v>1.0444444444444445</v>
+      </c>
+      <c r="O52" s="4">
+        <f t="shared" si="6"/>
+        <v>1.0444444444444445</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>52</v>
       </c>
@@ -2667,7 +2885,7 @@
         <v>45</v>
       </c>
       <c r="E53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>41</v>
       </c>
       <c r="F53">
@@ -2678,23 +2896,27 @@
         <v>1458</v>
       </c>
       <c r="H53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.48333333333333334</v>
       </c>
       <c r="I53">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24.3</v>
       </c>
       <c r="J53" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>24:18</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="2"/>
         <v>29:32</v>
       </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="O53" s="4">
+        <f t="shared" si="6"/>
+        <v>-1.0444444444444445</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>53</v>
       </c>
@@ -2705,7 +2927,7 @@
         <v>46</v>
       </c>
       <c r="E54">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>42</v>
       </c>
       <c r="F54">
@@ -2716,23 +2938,30 @@
         <v>1514</v>
       </c>
       <c r="H54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.93333333333333335</v>
       </c>
       <c r="I54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25.233333333333334</v>
       </c>
       <c r="J54" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>25:14</v>
       </c>
       <c r="K54" t="str">
         <f t="shared" si="2"/>
         <v>30:6</v>
       </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N54" s="5">
+        <v>1.0673611111111112</v>
+      </c>
+      <c r="O54" s="4">
+        <f t="shared" si="6"/>
+        <v>1.0673611111111112</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>54</v>
       </c>
@@ -2743,7 +2972,7 @@
         <v>47</v>
       </c>
       <c r="E55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>43</v>
       </c>
       <c r="F55">
@@ -2754,23 +2983,30 @@
         <v>1522</v>
       </c>
       <c r="H55">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.13333333333333333</v>
       </c>
       <c r="I55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25.366666666666667</v>
       </c>
       <c r="J55" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>25:22</v>
       </c>
       <c r="K55" t="str">
         <f t="shared" si="2"/>
         <v>30:40</v>
       </c>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N55" s="5">
+        <v>1.09375</v>
+      </c>
+      <c r="O55" s="4">
+        <f t="shared" si="6"/>
+        <v>2.6388888888888795E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>55</v>
       </c>
@@ -2781,7 +3017,7 @@
         <v>48</v>
       </c>
       <c r="E56">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>44</v>
       </c>
       <c r="F56">
@@ -2792,23 +3028,30 @@
         <v>1529</v>
       </c>
       <c r="H56">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.11666666666666667</v>
       </c>
       <c r="I56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25.483333333333334</v>
       </c>
       <c r="J56" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>25:29</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="2"/>
         <v>31:15</v>
       </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N56" s="5">
+        <v>1.0986111111111112</v>
+      </c>
+      <c r="O56" s="4">
+        <f t="shared" si="6"/>
+        <v>4.8611111111112049E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>56</v>
       </c>
@@ -2819,7 +3062,7 @@
         <v>49</v>
       </c>
       <c r="E57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="F57">
@@ -2830,23 +3073,30 @@
         <v>1542</v>
       </c>
       <c r="H57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.21666666666666667</v>
       </c>
       <c r="I57">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25.7</v>
       </c>
       <c r="J57" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>25:42</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="2"/>
         <v>31:49</v>
       </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N57" s="5">
+        <v>1.1020833333333333</v>
+      </c>
+      <c r="O57" s="4">
+        <f t="shared" si="6"/>
+        <v>3.4722222222220989E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>57</v>
       </c>
@@ -2857,7 +3107,7 @@
         <v>50</v>
       </c>
       <c r="E58">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>46</v>
       </c>
       <c r="F58">
@@ -2868,23 +3118,30 @@
         <v>1567</v>
       </c>
       <c r="H58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="I58">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26.116666666666667</v>
       </c>
       <c r="J58" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>26:7</v>
       </c>
       <c r="K58" t="str">
         <f t="shared" si="2"/>
         <v>32:23</v>
       </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N58" s="5">
+        <v>1.1125</v>
+      </c>
+      <c r="O58" s="4">
+        <f t="shared" si="6"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>58</v>
       </c>
@@ -2895,7 +3152,7 @@
         <v>51</v>
       </c>
       <c r="E59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>47</v>
       </c>
       <c r="F59">
@@ -2906,23 +3163,30 @@
         <v>1581</v>
       </c>
       <c r="H59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.23333333333333334</v>
       </c>
       <c r="I59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26.35</v>
       </c>
       <c r="J59" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>26:21</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="2"/>
         <v>32:57</v>
       </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N59" s="5">
+        <v>1.1333333333333333</v>
+      </c>
+      <c r="O59" s="4">
+        <f t="shared" si="6"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>59</v>
       </c>
@@ -2933,7 +3197,7 @@
         <v>52</v>
       </c>
       <c r="E60">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>48</v>
       </c>
       <c r="F60">
@@ -2944,23 +3208,28 @@
         <v>1623</v>
       </c>
       <c r="H60">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
       <c r="I60">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27.05</v>
       </c>
       <c r="J60" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>27:3</v>
       </c>
       <c r="K60" t="str">
         <f t="shared" si="2"/>
         <v>33:31</v>
       </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N60" s="5"/>
+      <c r="O60" s="4">
+        <f t="shared" si="6"/>
+        <v>-1.1333333333333333</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>60</v>
       </c>
@@ -2971,7 +3240,7 @@
         <v>53</v>
       </c>
       <c r="E61">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>49</v>
       </c>
       <c r="F61">
@@ -2982,23 +3251,30 @@
         <v>1648</v>
       </c>
       <c r="H61">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="I61">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27.466666666666665</v>
       </c>
       <c r="J61" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>27:27</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="2"/>
         <v>34:5</v>
       </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N61" s="5">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="O61" s="4">
+        <f t="shared" si="6"/>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>61</v>
       </c>
@@ -3009,7 +3285,7 @@
         <v>54</v>
       </c>
       <c r="E62">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="F62">
@@ -3020,23 +3296,28 @@
         <v>1668</v>
       </c>
       <c r="H62">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27.8</v>
       </c>
       <c r="J62" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>27:48</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="2"/>
         <v>34:39</v>
       </c>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N62" s="5"/>
+      <c r="O62" s="4">
+        <f t="shared" si="6"/>
+        <v>-1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>62</v>
       </c>
@@ -3047,7 +3328,7 @@
         <v>55</v>
       </c>
       <c r="E63">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>51</v>
       </c>
       <c r="F63">
@@ -3058,23 +3339,30 @@
         <v>1681</v>
       </c>
       <c r="H63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.21666666666666667</v>
       </c>
       <c r="I63">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28.016666666666666</v>
       </c>
       <c r="J63" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>28:0</v>
       </c>
       <c r="K63" t="str">
         <f t="shared" si="2"/>
         <v>35:13</v>
       </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N63" s="5">
+        <v>1.2013888888888888</v>
+      </c>
+      <c r="O63" s="4">
+        <f t="shared" si="6"/>
+        <v>1.2013888888888888</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>63</v>
       </c>
@@ -3085,7 +3373,7 @@
         <v>56</v>
       </c>
       <c r="E64">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>52</v>
       </c>
       <c r="F64">
@@ -3096,15 +3384,15 @@
         <v>1701</v>
       </c>
       <c r="H64">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28.35</v>
       </c>
       <c r="J64" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>28:21</v>
       </c>
       <c r="K64" t="str">
@@ -3112,7 +3400,7 @@
         <v>35:47</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>64</v>
       </c>
@@ -3123,7 +3411,7 @@
         <v>57</v>
       </c>
       <c r="E65">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>53</v>
       </c>
       <c r="F65">
@@ -3134,15 +3422,15 @@
         <v>1721</v>
       </c>
       <c r="H65">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I65">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28.683333333333334</v>
       </c>
       <c r="J65" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>28:41</v>
       </c>
       <c r="K65" t="str">
@@ -3150,7 +3438,7 @@
         <v>36:21</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>65</v>
       </c>
@@ -3161,7 +3449,7 @@
         <v>58</v>
       </c>
       <c r="E66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>54</v>
       </c>
       <c r="F66">
@@ -3172,23 +3460,23 @@
         <v>1741</v>
       </c>
       <c r="H66">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I66">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29.016666666666666</v>
       </c>
       <c r="J66" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>29:0</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" ref="K66:K89" si="17">INT($A$2*B66)&amp;":"&amp;TEXT(INT(($A$2*B66-INT($A$2*B66))*60),0)</f>
+        <f t="shared" si="2"/>
         <v>36:55</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>66</v>
       </c>
@@ -3199,7 +3487,7 @@
         <v>59</v>
       </c>
       <c r="E67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>55</v>
       </c>
       <c r="F67">
@@ -3210,23 +3498,26 @@
         <v>1761</v>
       </c>
       <c r="H67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I67">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29.35</v>
       </c>
       <c r="J67" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="J67:J89" si="14">INT(I67)&amp;":"&amp;INT((I67-INT(I67))*60)</f>
         <v>29:21</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="K67:K89" si="15">INT($A$2*B67)&amp;":"&amp;TEXT(INT(($A$2*B67-INT($A$2*B67))*60),0)</f>
         <v>37:30</v>
       </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="P67" s="5">
+        <v>1.3125</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>67</v>
       </c>
@@ -3237,34 +3528,34 @@
         <v>60</v>
       </c>
       <c r="E68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>56</v>
       </c>
       <c r="F68">
         <v>20</v>
       </c>
       <c r="G68">
-        <f t="shared" ref="G68:G89" si="18">F68+G67</f>
+        <f t="shared" ref="G68:G89" si="16">F68+G67</f>
         <v>1781</v>
       </c>
       <c r="H68">
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="13"/>
+        <v>29.683333333333334</v>
+      </c>
+      <c r="J68" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I68">
+        <v>29:41</v>
+      </c>
+      <c r="K68" t="str">
         <f t="shared" si="15"/>
-        <v>29.683333333333334</v>
-      </c>
-      <c r="J68" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>29:41</v>
-      </c>
-      <c r="K68" t="str">
-        <f t="shared" si="17"/>
         <v>38:4</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>68</v>
       </c>
@@ -3275,34 +3566,34 @@
         <v>61</v>
       </c>
       <c r="E69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>57</v>
       </c>
       <c r="F69">
         <v>10</v>
       </c>
       <c r="G69">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1791</v>
       </c>
       <c r="H69">
+        <f t="shared" si="12"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="13"/>
+        <v>29.85</v>
+      </c>
+      <c r="J69" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="I69">
+        <v>29:51</v>
+      </c>
+      <c r="K69" t="str">
         <f t="shared" si="15"/>
-        <v>29.85</v>
-      </c>
-      <c r="J69" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>29:51</v>
-      </c>
-      <c r="K69" t="str">
-        <f t="shared" si="17"/>
         <v>38:38</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>69</v>
       </c>
@@ -3313,34 +3604,34 @@
         <v>62</v>
       </c>
       <c r="E70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>58</v>
       </c>
       <c r="F70">
         <v>12</v>
       </c>
       <c r="G70">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1803</v>
       </c>
       <c r="H70">
+        <f t="shared" si="12"/>
+        <v>0.2</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="13"/>
+        <v>30.05</v>
+      </c>
+      <c r="J70" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.2</v>
-      </c>
-      <c r="I70">
+        <v>30:3</v>
+      </c>
+      <c r="K70" t="str">
         <f t="shared" si="15"/>
-        <v>30.05</v>
-      </c>
-      <c r="J70" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>30:3</v>
-      </c>
-      <c r="K70" t="str">
-        <f t="shared" si="17"/>
         <v>39:12</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>70</v>
       </c>
@@ -3351,34 +3642,34 @@
         <v>63</v>
       </c>
       <c r="E71">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>59</v>
       </c>
       <c r="F71">
         <v>23</v>
       </c>
       <c r="G71">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1826</v>
       </c>
       <c r="H71">
+        <f t="shared" si="12"/>
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="13"/>
+        <v>30.433333333333334</v>
+      </c>
+      <c r="J71" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.38333333333333336</v>
-      </c>
-      <c r="I71">
+        <v>30:26</v>
+      </c>
+      <c r="K71" t="str">
         <f t="shared" si="15"/>
-        <v>30.433333333333334</v>
-      </c>
-      <c r="J71" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>30:26</v>
-      </c>
-      <c r="K71" t="str">
-        <f t="shared" si="17"/>
         <v>39:46</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>71</v>
       </c>
@@ -3389,34 +3680,34 @@
         <v>64</v>
       </c>
       <c r="E72">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="F72">
         <v>20</v>
       </c>
       <c r="G72">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1846</v>
       </c>
       <c r="H72">
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="13"/>
+        <v>30.766666666666666</v>
+      </c>
+      <c r="J72" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I72">
+        <v>30:45</v>
+      </c>
+      <c r="K72" t="str">
         <f t="shared" si="15"/>
-        <v>30.766666666666666</v>
-      </c>
-      <c r="J72" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>30:45</v>
-      </c>
-      <c r="K72" t="str">
-        <f t="shared" si="17"/>
         <v>40:20</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>72</v>
       </c>
@@ -3427,34 +3718,34 @@
         <v>65</v>
       </c>
       <c r="E73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>61</v>
       </c>
       <c r="F73">
         <v>25</v>
       </c>
       <c r="G73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1871</v>
       </c>
       <c r="H73">
+        <f t="shared" si="12"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="13"/>
+        <v>31.183333333333334</v>
+      </c>
+      <c r="J73" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="I73">
+        <v>31:11</v>
+      </c>
+      <c r="K73" t="str">
         <f t="shared" si="15"/>
-        <v>31.183333333333334</v>
-      </c>
-      <c r="J73" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>31:11</v>
-      </c>
-      <c r="K73" t="str">
-        <f t="shared" si="17"/>
         <v>40:54</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>73</v>
       </c>
@@ -3465,34 +3756,34 @@
         <v>66</v>
       </c>
       <c r="E74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>62</v>
       </c>
       <c r="F74">
         <v>20</v>
       </c>
       <c r="G74">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1891</v>
       </c>
       <c r="H74">
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="13"/>
+        <v>31.516666666666666</v>
+      </c>
+      <c r="J74" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I74">
+        <v>31:30</v>
+      </c>
+      <c r="K74" t="str">
         <f t="shared" si="15"/>
-        <v>31.516666666666666</v>
-      </c>
-      <c r="J74" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>31:30</v>
-      </c>
-      <c r="K74" t="str">
-        <f t="shared" si="17"/>
         <v>41:28</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>74</v>
       </c>
@@ -3503,34 +3794,34 @@
         <v>67</v>
       </c>
       <c r="E75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>63</v>
       </c>
       <c r="F75">
         <v>27</v>
       </c>
       <c r="G75">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1918</v>
       </c>
       <c r="H75">
+        <f t="shared" si="12"/>
+        <v>0.45</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="13"/>
+        <v>31.966666666666665</v>
+      </c>
+      <c r="J75" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.45</v>
-      </c>
-      <c r="I75">
+        <v>31:57</v>
+      </c>
+      <c r="K75" t="str">
         <f t="shared" si="15"/>
-        <v>31.966666666666665</v>
-      </c>
-      <c r="J75" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>31:57</v>
-      </c>
-      <c r="K75" t="str">
-        <f t="shared" si="17"/>
         <v>42:2</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>75</v>
       </c>
@@ -3541,34 +3832,34 @@
         <v>68</v>
       </c>
       <c r="E76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="F76">
         <v>25</v>
       </c>
       <c r="G76">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1943</v>
       </c>
       <c r="H76">
+        <f t="shared" si="12"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="13"/>
+        <v>32.383333333333333</v>
+      </c>
+      <c r="J76" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="I76">
+        <v>32:23</v>
+      </c>
+      <c r="K76" t="str">
         <f t="shared" si="15"/>
-        <v>32.383333333333333</v>
-      </c>
-      <c r="J76" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>32:23</v>
-      </c>
-      <c r="K76" t="str">
-        <f t="shared" si="17"/>
         <v>42:36</v>
       </c>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>76</v>
       </c>
@@ -3579,34 +3870,34 @@
         <v>69</v>
       </c>
       <c r="E77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>65</v>
       </c>
       <c r="F77">
         <v>36</v>
       </c>
       <c r="G77">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1979</v>
       </c>
       <c r="H77">
+        <f t="shared" si="12"/>
+        <v>0.6</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="13"/>
+        <v>32.983333333333334</v>
+      </c>
+      <c r="J77" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.6</v>
-      </c>
-      <c r="I77">
+        <v>32:59</v>
+      </c>
+      <c r="K77" t="str">
         <f t="shared" si="15"/>
-        <v>32.983333333333334</v>
-      </c>
-      <c r="J77" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>32:59</v>
-      </c>
-      <c r="K77" t="str">
-        <f t="shared" si="17"/>
         <v>43:10</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>77</v>
       </c>
@@ -3617,34 +3908,34 @@
         <v>70</v>
       </c>
       <c r="E78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>65</v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
       <c r="G78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1979</v>
       </c>
       <c r="H78">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="13"/>
+        <v>32.983333333333334</v>
+      </c>
+      <c r="J78" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="I78">
+        <v>32:59</v>
+      </c>
+      <c r="K78" t="str">
         <f t="shared" si="15"/>
-        <v>32.983333333333334</v>
-      </c>
-      <c r="J78" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>32:59</v>
-      </c>
-      <c r="K78" t="str">
-        <f t="shared" si="17"/>
         <v>43:45</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>78</v>
       </c>
@@ -3655,34 +3946,34 @@
         <v>71</v>
       </c>
       <c r="E79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>66</v>
       </c>
       <c r="F79">
         <v>13</v>
       </c>
       <c r="G79">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>1992</v>
       </c>
       <c r="H79">
+        <f t="shared" si="12"/>
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="13"/>
+        <v>33.200000000000003</v>
+      </c>
+      <c r="J79" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.21666666666666667</v>
-      </c>
-      <c r="I79">
+        <v>33:12</v>
+      </c>
+      <c r="K79" t="str">
         <f t="shared" si="15"/>
-        <v>33.200000000000003</v>
-      </c>
-      <c r="J79" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>33:12</v>
-      </c>
-      <c r="K79" t="str">
-        <f t="shared" si="17"/>
         <v>44:19</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>79</v>
       </c>
@@ -3693,34 +3984,34 @@
         <v>72</v>
       </c>
       <c r="E80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>67</v>
       </c>
       <c r="F80">
         <v>53</v>
       </c>
       <c r="G80">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2045</v>
       </c>
       <c r="H80">
+        <f t="shared" si="12"/>
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="13"/>
+        <v>34.083333333333336</v>
+      </c>
+      <c r="J80" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.8833333333333333</v>
-      </c>
-      <c r="I80">
+        <v>34:5</v>
+      </c>
+      <c r="K80" t="str">
         <f t="shared" si="15"/>
-        <v>34.083333333333336</v>
-      </c>
-      <c r="J80" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>34:5</v>
-      </c>
-      <c r="K80" t="str">
-        <f t="shared" si="17"/>
         <v>44:53</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>80</v>
       </c>
@@ -3731,34 +4022,34 @@
         <v>73</v>
       </c>
       <c r="E81">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>68</v>
       </c>
       <c r="F81">
         <v>15</v>
       </c>
       <c r="G81">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2060</v>
       </c>
       <c r="H81">
+        <f t="shared" si="12"/>
+        <v>0.25</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="13"/>
+        <v>34.333333333333336</v>
+      </c>
+      <c r="J81" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>0.25</v>
-      </c>
-      <c r="I81">
+        <v>34:20</v>
+      </c>
+      <c r="K81" t="str">
         <f t="shared" si="15"/>
-        <v>34.333333333333336</v>
-      </c>
-      <c r="J81" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>34:20</v>
-      </c>
-      <c r="K81" t="str">
-        <f t="shared" si="17"/>
         <v>45:27</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>81</v>
       </c>
@@ -3769,34 +4060,34 @@
         <v>74</v>
       </c>
       <c r="E82">
-        <f t="shared" ref="E82:E89" si="19">IF(NOT(OR(C82="Agenda",C82="Final",D82=D81)),E81+1,E81+0)</f>
+        <f t="shared" ref="E82:E89" si="17">IF(NOT(OR(C82="Agenda",C82="Final",D82=D81)),E81+1,E81+0)</f>
         <v>69</v>
       </c>
       <c r="F82">
         <v>8</v>
       </c>
       <c r="G82">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2068</v>
       </c>
       <c r="H82">
-        <f t="shared" ref="H82:H89" si="20">F82/60</f>
+        <f t="shared" ref="H82:H89" si="18">F82/60</f>
         <v>0.13333333333333333</v>
       </c>
       <c r="I82">
-        <f t="shared" ref="I82:I89" si="21">G82/60</f>
+        <f t="shared" ref="I82:I89" si="19">G82/60</f>
         <v>34.466666666666669</v>
       </c>
       <c r="J82" s="2" t="str">
-        <f t="shared" ref="J82:J89" si="22">INT(I82)&amp;":"&amp;INT((I82-INT(I82))*60)</f>
+        <f t="shared" si="14"/>
         <v>34:28</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>46:1</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>82</v>
       </c>
@@ -3807,34 +4098,34 @@
         <v>75</v>
       </c>
       <c r="E83">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>70</v>
       </c>
       <c r="F83">
         <v>45</v>
       </c>
       <c r="G83">
+        <f t="shared" si="16"/>
+        <v>2113</v>
+      </c>
+      <c r="H83">
         <f t="shared" si="18"/>
-        <v>2113</v>
-      </c>
-      <c r="H83">
-        <f t="shared" si="20"/>
         <v>0.75</v>
       </c>
       <c r="I83">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>35.216666666666669</v>
       </c>
       <c r="J83" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>35:13</v>
       </c>
       <c r="K83" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>46:35</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>83</v>
       </c>
@@ -3845,34 +4136,34 @@
         <v>76</v>
       </c>
       <c r="E84">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>71</v>
       </c>
       <c r="F84">
         <v>17</v>
       </c>
       <c r="G84">
+        <f t="shared" si="16"/>
+        <v>2130</v>
+      </c>
+      <c r="H84">
         <f t="shared" si="18"/>
-        <v>2130</v>
-      </c>
-      <c r="H84">
-        <f t="shared" si="20"/>
         <v>0.28333333333333333</v>
       </c>
       <c r="I84">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>35.5</v>
       </c>
       <c r="J84" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>35:30</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>47:9</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>84</v>
       </c>
@@ -3883,34 +4174,34 @@
         <v>77</v>
       </c>
       <c r="E85">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>72</v>
       </c>
       <c r="F85">
         <v>11</v>
       </c>
       <c r="G85">
+        <f t="shared" si="16"/>
+        <v>2141</v>
+      </c>
+      <c r="H85">
         <f t="shared" si="18"/>
-        <v>2141</v>
-      </c>
-      <c r="H85">
-        <f t="shared" si="20"/>
         <v>0.18333333333333332</v>
       </c>
       <c r="I85">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>35.68333333333333</v>
       </c>
       <c r="J85" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>35:40</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>47:43</v>
       </c>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>85</v>
       </c>
@@ -3921,34 +4212,34 @@
         <v>78</v>
       </c>
       <c r="E86">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>73</v>
       </c>
       <c r="F86">
         <v>8</v>
       </c>
       <c r="G86">
+        <f t="shared" si="16"/>
+        <v>2149</v>
+      </c>
+      <c r="H86">
         <f t="shared" si="18"/>
-        <v>2149</v>
-      </c>
-      <c r="H86">
-        <f t="shared" si="20"/>
         <v>0.13333333333333333</v>
       </c>
       <c r="I86">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>35.81666666666667</v>
       </c>
       <c r="J86" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>35:49</v>
       </c>
       <c r="K86" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>48:17</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>86</v>
       </c>
@@ -3959,34 +4250,34 @@
         <v>79</v>
       </c>
       <c r="E87">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>74</v>
       </c>
       <c r="F87">
         <v>10</v>
       </c>
       <c r="G87">
+        <f t="shared" si="16"/>
+        <v>2159</v>
+      </c>
+      <c r="H87">
         <f t="shared" si="18"/>
-        <v>2159</v>
-      </c>
-      <c r="H87">
-        <f t="shared" si="20"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="I87">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>35.983333333333334</v>
       </c>
       <c r="J87" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>35:59</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>48:51</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>87</v>
       </c>
@@ -3997,34 +4288,34 @@
         <v>80</v>
       </c>
       <c r="E88">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>75</v>
       </c>
       <c r="F88">
         <v>10</v>
       </c>
       <c r="G88">
+        <f t="shared" si="16"/>
+        <v>2169</v>
+      </c>
+      <c r="H88">
         <f t="shared" si="18"/>
-        <v>2169</v>
-      </c>
-      <c r="H88">
-        <f t="shared" si="20"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="I88">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>36.15</v>
       </c>
       <c r="J88" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>36:8</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>49:25</v>
       </c>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>88</v>
       </c>
@@ -4035,31 +4326,34 @@
         <v>81</v>
       </c>
       <c r="E89">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>75</v>
       </c>
       <c r="F89">
         <v>10</v>
       </c>
       <c r="G89">
+        <f t="shared" si="16"/>
+        <v>2179</v>
+      </c>
+      <c r="H89">
         <f t="shared" si="18"/>
-        <v>2179</v>
-      </c>
-      <c r="H89">
-        <f t="shared" si="20"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="I89">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>36.31666666666667</v>
       </c>
       <c r="J89" s="2" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="14"/>
         <v>36:19</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>50:0</v>
+      </c>
+      <c r="P89">
+        <v>40</v>
       </c>
     </row>
     <row r="1048575" spans="14:14" x14ac:dyDescent="0.25">

</xml_diff>